<commit_message>
corrected error in transitor count calculation; added more data points to regression calculation and saved them excel file; added script to calculate shifted tanh from 1991 PLA of logistic function; added function to calculate coefficients for polynomial regression
</commit_message>
<xml_diff>
--- a/Matlab/Chebyshev/FPGA_Ressources/ALM_DSP_WORDLENGTH_pairs.xlsx
+++ b/Matlab/Chebyshev/FPGA_Ressources/ALM_DSP_WORDLENGTH_pairs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>combined wordlength</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>CL</t>
+  </si>
+  <si>
+    <t>total registers</t>
   </si>
 </sst>
 </file>
@@ -359,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,7 +376,7 @@
     <col min="6" max="6" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -392,8 +395,11 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -414,7 +420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -435,7 +441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -456,7 +462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8</v>
       </c>
@@ -476,7 +482,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -496,7 +502,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>12</v>
       </c>
@@ -516,7 +522,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>16</v>
       </c>
@@ -536,7 +542,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>32</v>
       </c>
@@ -556,7 +562,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>24</v>
       </c>
@@ -576,7 +582,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>32</v>
       </c>
@@ -594,6 +600,1041 @@
       </c>
       <c r="F11">
         <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>11</v>
+      </c>
+      <c r="G16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>13</v>
+      </c>
+      <c r="G18">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>13</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>14</v>
+      </c>
+      <c r="G19">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>15</v>
+      </c>
+      <c r="G20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>16</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>17</v>
+      </c>
+      <c r="G21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>18</v>
+      </c>
+      <c r="D22">
+        <v>16</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>17</v>
+      </c>
+      <c r="G22">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>17</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>18</v>
+      </c>
+      <c r="G23">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>22</v>
+      </c>
+      <c r="D24">
+        <v>19</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>20</v>
+      </c>
+      <c r="G24">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>22</v>
+      </c>
+      <c r="D25">
+        <v>19</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+      <c r="G25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+      <c r="D26">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>21</v>
+      </c>
+      <c r="G26">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>22</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>23</v>
+      </c>
+      <c r="G27">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28">
+        <v>14</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <v>23</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>24</v>
+      </c>
+      <c r="G28">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <v>24</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>25</v>
+      </c>
+      <c r="G29">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>14</v>
+      </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+      <c r="D30">
+        <v>26</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>27</v>
+      </c>
+      <c r="G30">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>16</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <v>27</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>28</v>
+      </c>
+      <c r="G31">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>32</v>
+      </c>
+      <c r="D32">
+        <v>27</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>28</v>
+      </c>
+      <c r="G32">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>18</v>
+      </c>
+      <c r="B33">
+        <v>16</v>
+      </c>
+      <c r="C33">
+        <v>34</v>
+      </c>
+      <c r="D33">
+        <v>29</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>30</v>
+      </c>
+      <c r="G33">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>16</v>
+      </c>
+      <c r="B34">
+        <v>18</v>
+      </c>
+      <c r="C34">
+        <v>34</v>
+      </c>
+      <c r="D34">
+        <v>30</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>31</v>
+      </c>
+      <c r="G34">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>18</v>
+      </c>
+      <c r="C35">
+        <v>36</v>
+      </c>
+      <c r="D35">
+        <v>32</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>33</v>
+      </c>
+      <c r="G35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>20</v>
+      </c>
+      <c r="B36">
+        <v>18</v>
+      </c>
+      <c r="C36">
+        <v>38</v>
+      </c>
+      <c r="D36">
+        <v>46</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>48</v>
+      </c>
+      <c r="G36">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>18</v>
+      </c>
+      <c r="B37">
+        <v>20</v>
+      </c>
+      <c r="C37">
+        <v>38</v>
+      </c>
+      <c r="D37">
+        <v>46</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>48</v>
+      </c>
+      <c r="G37">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>20</v>
+      </c>
+      <c r="B38">
+        <v>20</v>
+      </c>
+      <c r="C38">
+        <v>40</v>
+      </c>
+      <c r="D38">
+        <v>49</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>51</v>
+      </c>
+      <c r="G38">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>22</v>
+      </c>
+      <c r="B39">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <v>42</v>
+      </c>
+      <c r="D39">
+        <v>52</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>54</v>
+      </c>
+      <c r="G39">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>20</v>
+      </c>
+      <c r="B40">
+        <v>22</v>
+      </c>
+      <c r="C40">
+        <v>42</v>
+      </c>
+      <c r="D40">
+        <v>52</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>54</v>
+      </c>
+      <c r="G40">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>22</v>
+      </c>
+      <c r="B41">
+        <v>22</v>
+      </c>
+      <c r="C41">
+        <v>44</v>
+      </c>
+      <c r="D41">
+        <v>55</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>57</v>
+      </c>
+      <c r="G41">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>24</v>
+      </c>
+      <c r="B42">
+        <v>22</v>
+      </c>
+      <c r="C42">
+        <v>46</v>
+      </c>
+      <c r="D42">
+        <v>58</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>60</v>
+      </c>
+      <c r="G42">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>22</v>
+      </c>
+      <c r="B43">
+        <v>24</v>
+      </c>
+      <c r="C43">
+        <v>46</v>
+      </c>
+      <c r="D43">
+        <v>58</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>60</v>
+      </c>
+      <c r="G43">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>24</v>
+      </c>
+      <c r="B44">
+        <v>24</v>
+      </c>
+      <c r="C44">
+        <v>48</v>
+      </c>
+      <c r="D44">
+        <v>61</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>63</v>
+      </c>
+      <c r="G44">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>26</v>
+      </c>
+      <c r="B45">
+        <v>24</v>
+      </c>
+      <c r="C45">
+        <v>50</v>
+      </c>
+      <c r="D45">
+        <v>64</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>66</v>
+      </c>
+      <c r="G45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>26</v>
+      </c>
+      <c r="C46">
+        <v>50</v>
+      </c>
+      <c r="D46">
+        <v>64</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>66</v>
+      </c>
+      <c r="G46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>26</v>
+      </c>
+      <c r="B47">
+        <v>26</v>
+      </c>
+      <c r="C47">
+        <v>52</v>
+      </c>
+      <c r="D47">
+        <v>67</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>69</v>
+      </c>
+      <c r="G47">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>28</v>
+      </c>
+      <c r="B48">
+        <v>26</v>
+      </c>
+      <c r="C48">
+        <v>54</v>
+      </c>
+      <c r="D48">
+        <v>70</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48">
+        <v>74</v>
+      </c>
+      <c r="G48">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>26</v>
+      </c>
+      <c r="B49">
+        <v>28</v>
+      </c>
+      <c r="C49">
+        <v>54</v>
+      </c>
+      <c r="D49">
+        <v>70</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>72</v>
+      </c>
+      <c r="G49">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>28</v>
+      </c>
+      <c r="B50">
+        <v>28</v>
+      </c>
+      <c r="C50">
+        <v>56</v>
+      </c>
+      <c r="D50">
+        <v>73</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>77</v>
+      </c>
+      <c r="G50">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>30</v>
+      </c>
+      <c r="B51">
+        <v>28</v>
+      </c>
+      <c r="C51">
+        <v>58</v>
+      </c>
+      <c r="D51">
+        <v>76</v>
+      </c>
+      <c r="E51">
+        <v>4</v>
+      </c>
+      <c r="F51">
+        <v>80</v>
+      </c>
+      <c r="G51">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>28</v>
+      </c>
+      <c r="B52">
+        <v>30</v>
+      </c>
+      <c r="C52">
+        <v>58</v>
+      </c>
+      <c r="D52">
+        <v>76</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+      <c r="F52">
+        <v>80</v>
+      </c>
+      <c r="G52">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>30</v>
+      </c>
+      <c r="B53">
+        <v>30</v>
+      </c>
+      <c r="C53">
+        <v>60</v>
+      </c>
+      <c r="D53">
+        <v>79</v>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+      <c r="F53">
+        <v>83</v>
+      </c>
+      <c r="G53">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>32</v>
+      </c>
+      <c r="B54">
+        <v>30</v>
+      </c>
+      <c r="C54">
+        <v>62</v>
+      </c>
+      <c r="D54">
+        <v>82</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54">
+        <v>86</v>
+      </c>
+      <c r="G54">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>30</v>
+      </c>
+      <c r="B55">
+        <v>32</v>
+      </c>
+      <c r="C55">
+        <v>62</v>
+      </c>
+      <c r="D55">
+        <v>82</v>
+      </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
+      <c r="F55">
+        <v>86</v>
+      </c>
+      <c r="G55">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>32</v>
+      </c>
+      <c r="B56">
+        <v>32</v>
+      </c>
+      <c r="C56">
+        <v>64</v>
+      </c>
+      <c r="D56">
+        <v>90</v>
+      </c>
+      <c r="E56">
+        <v>6</v>
+      </c>
+      <c r="F56">
+        <v>96</v>
+      </c>
+      <c r="G56">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>